<commit_message>
Minor update: Just checking whether this works with .xlsx
</commit_message>
<xml_diff>
--- a/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
+++ b/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="120" windowWidth="10500" windowHeight="9000" activeTab="3"/>
+    <workbookView xWindow="285" yWindow="120" windowWidth="10500" windowHeight="9000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Schermen" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1039" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="285">
   <si>
     <t>Scherm</t>
   </si>
@@ -855,9 +855,6 @@
   </si>
   <si>
     <t>Verstuur naar P-Direct</t>
-  </si>
-  <si>
-    <t>conditie</t>
   </si>
   <si>
     <t>Actie</t>
@@ -907,6 +904,18 @@
     <t>Het verwerken door de kennismotor gaat per periodeverantwoording. Het is niet noodzakelijk om alle periodeverantwoordingen in één enkele transactie door de kennismotor te halen. De kennismotor moet net zolang worden aangeroepen, totdat er geen periodeverantwoording meer is met de status 'te verwerken'. 
 Zolang de kennismotor loopt, moet het duidelijk zijn voor de gebruiker dat er op de achtergrond wordt gewerkt. Dat kan bijvoorbeeld zijn door de tellertjes bij te werken in het scherm, maar mag ook anders worden opgelost. 
 Indien tijdens het verwerken op vernieuwen vanuit Spin wordt gedrukt, dan mag de kennismotor worden gestopt. Immers, zowel de nog niet verwerkte periodeverantwoordingen als ook de periodeverantwoordingen die door de kennismotor zijn verwerkt, zullen worden verwijderd.</t>
+  </si>
+  <si>
+    <t>activeringsEvent</t>
+  </si>
+  <si>
+    <t>activeringsConditie</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Klik op knop</t>
   </si>
 </sst>
 </file>
@@ -1286,17 +1295,17 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" customWidth="1"/>
-    <col min="4" max="4" width="64.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="64.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1328,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1339,7 +1348,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1379,7 +1388,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1396,7 +1405,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1416,7 +1425,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1476,7 +1485,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1493,7 +1502,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1510,7 +1519,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1525,7 +1534,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1542,7 +1551,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1562,7 +1571,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1582,7 +1591,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1597,7 +1606,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1651,7 +1660,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1671,7 +1680,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1696,7 +1705,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1713,7 +1722,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1733,7 +1742,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1747,7 +1756,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1764,7 +1773,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1803,16 +1812,16 @@
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="48.88671875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="6" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -1841,7 +1850,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1867,7 +1876,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1893,7 +1902,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1910,7 +1919,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1933,7 +1942,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1956,7 +1965,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1987,7 +1996,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2010,7 +2019,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2033,7 +2042,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -2102,7 +2111,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2125,7 +2134,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -2148,7 +2157,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2188,7 +2197,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -2248,7 +2257,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -2271,7 +2280,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -2291,7 +2300,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2311,7 +2320,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -2331,7 +2340,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2348,7 +2357,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -2371,7 +2380,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -2394,7 +2403,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -2414,7 +2423,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -2434,7 +2443,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -2457,7 +2466,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -2477,7 +2486,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2497,7 +2506,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2563,7 +2572,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2586,7 +2595,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -2626,7 +2635,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2649,7 +2658,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -2672,7 +2681,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -2695,7 +2704,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -2718,7 +2727,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>141</v>
       </c>
@@ -2741,7 +2750,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -2764,7 +2773,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>146</v>
       </c>
@@ -2787,7 +2796,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -2810,7 +2819,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>151</v>
       </c>
@@ -2836,7 +2845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2859,7 +2868,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -2882,7 +2891,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -2911,7 +2920,7 @@
         <v>5010</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -2937,7 +2946,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>208</v>
       </c>
@@ -2960,7 +2969,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>162</v>
       </c>
@@ -2983,7 +2992,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -3000,7 +3009,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>165</v>
       </c>
@@ -3023,7 +3032,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>167</v>
       </c>
@@ -3053,25 +3062,25 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="864" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="870" topLeftCell="A16" activePane="bottomLeft"/>
       <selection sqref="A1:XFD2"/>
       <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.21875" customWidth="1"/>
-    <col min="8" max="8" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -3109,7 +3118,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3141,7 +3150,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -3167,7 +3176,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -3193,7 +3202,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -3222,7 +3231,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -3251,7 +3260,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -3286,7 +3295,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3318,7 +3327,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -3350,7 +3359,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -3382,7 +3391,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -3414,7 +3423,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -3446,7 +3455,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>226</v>
       </c>
@@ -3472,7 +3481,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>210</v>
       </c>
@@ -3504,7 +3513,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -3536,7 +3545,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -3571,7 +3580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>227</v>
       </c>
@@ -3600,7 +3609,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>228</v>
       </c>
@@ -3629,7 +3638,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>229</v>
       </c>
@@ -3658,7 +3667,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>231</v>
       </c>
@@ -3693,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>5010</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -3777,7 +3786,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -3809,7 +3818,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>233</v>
       </c>
@@ -3838,7 +3847,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>165</v>
       </c>
@@ -3870,7 +3879,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>167</v>
       </c>
@@ -3899,7 +3908,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>240</v>
       </c>
@@ -3922,7 +3931,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>185</v>
       </c>
@@ -3948,7 +3957,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>185</v>
       </c>
@@ -3974,7 +3983,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>185</v>
       </c>
@@ -4000,7 +4009,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>185</v>
       </c>
@@ -4026,7 +4035,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>185</v>
       </c>
@@ -4052,7 +4061,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>185</v>
       </c>
@@ -4078,7 +4087,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>185</v>
       </c>
@@ -4104,7 +4113,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>200</v>
       </c>
@@ -4130,7 +4139,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>200</v>
       </c>
@@ -4156,7 +4165,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>201</v>
       </c>
@@ -4179,7 +4188,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>201</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>202</v>
       </c>
@@ -4228,7 +4237,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>203</v>
       </c>
@@ -4251,7 +4260,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>203</v>
       </c>
@@ -4274,7 +4283,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>203</v>
       </c>
@@ -4297,7 +4306,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>203</v>
       </c>
@@ -4323,7 +4332,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>203</v>
       </c>
@@ -4349,7 +4358,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>203</v>
       </c>
@@ -4375,7 +4384,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>206</v>
       </c>
@@ -4401,7 +4410,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>206</v>
       </c>
@@ -4427,7 +4436,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>206</v>
       </c>
@@ -4453,7 +4462,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>206</v>
       </c>
@@ -4479,7 +4488,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>206</v>
       </c>
@@ -4505,7 +4514,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>206</v>
       </c>
@@ -4531,7 +4540,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>206</v>
       </c>
@@ -4568,21 +4577,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.21875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="20.28515625" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -4596,10 +4605,10 @@
         <v>262</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>77</v>
       </c>
@@ -4650,7 +4659,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4709,113 +4718,127 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="40.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="40.5546875" style="4"/>
+    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="58.5703125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="40.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>267</v>
-      </c>
       <c r="B2" s="4" t="s">
-        <v>267</v>
+        <v>283</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="288" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>272</v>
-      </c>
       <c r="C4" s="4" t="s">
         <v>271</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="E4" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="E5" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>275</v>
-      </c>
       <c r="C6" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some more stuff for Han
</commit_message>
<xml_diff>
--- a/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
+++ b/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="285" yWindow="120" windowWidth="10500" windowHeight="9000" activeTab="4"/>
+    <workbookView xWindow="288" yWindow="120" windowWidth="10500" windowHeight="9000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Schermen" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="306">
   <si>
     <t>Scherm</t>
   </si>
@@ -851,16 +851,10 @@
     <t>er bestaan periodeverantwoordingen met status 'uitval'</t>
   </si>
   <si>
-    <t>Vernieuw vanuit Spin</t>
-  </si>
-  <si>
     <t>Verstuur naar P-Direct</t>
   </si>
   <si>
     <t>Actie</t>
-  </si>
-  <si>
-    <t>Verwijder alle periodeverantwoordingen die NIET de status 'verzonden' hebben uit DTV. Haal daarna de nieuwe batch op uit SPIN</t>
   </si>
   <si>
     <t>beschrijving</t>
@@ -883,19 +877,6 @@
   </si>
   <si>
     <t>Er is géén periodeverantwoording met de status 'te verwerken'</t>
-  </si>
-  <si>
-    <t>De terugkoppelberichten voor medewerkers en teamleiders worden vrijgegeven via een signaal naar het datawarehouse.</t>
-  </si>
-  <si>
-    <t>Het idee is dat dit signaal aan het datawarehouse er toe leidt, dat de medewerkers die te corrigeren periodeverantwoordingen hebben, daarvan in kennis worden gesteld.</t>
-  </si>
-  <si>
-    <t>Maak een P-Direct bestand aan, waarin alle periodeverantwoordingen worden opgenomen met de status 'te verzenden'. Die periodeverantwoordingen krijgen de status 'verzonden'. 
-Verwijder aansluitend alle periodeverantwoordingen die NIET de status 'verzonden' hebben uit DTV.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Het aanmaken van het bestand is een atomaire actie, zodat precies bekend is welke periodeverantwoordingen zijn opgenomen. </t>
   </si>
   <si>
     <t>Rollen</t>
@@ -915,14 +896,96 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Klik op knop</t>
+    <t>Knop</t>
+  </si>
+  <si>
+    <t>[Knoppen]</t>
+  </si>
+  <si>
+    <t>KNOP-1</t>
+  </si>
+  <si>
+    <t>KNOP-2</t>
+  </si>
+  <si>
+    <t>KNOP-3</t>
+  </si>
+  <si>
+    <t>Vernieuw alle periodeverantwoordingen</t>
+  </si>
+  <si>
+    <t>KNOP-4</t>
+  </si>
+  <si>
+    <t>Klik</t>
+  </si>
+  <si>
+    <t>Het tijdstip van de klik wordt in een record opgeslagen, wat periodiek door SAS wordt uitgelezen. SAS stelt aan de hand van deze datum vast dat er nieuwe verantwoordingen klaarstaan. SAS zal de terugkoppelberichten voor medewerkers en teamleiders zelf uitlezen.</t>
+  </si>
+  <si>
+    <t>Maak een P-Direct bestand aan, waarin alle periodeverantwoordingen worden verwerkt met de status 'te verzenden'. Die periodeverantwoordingen krijgen de status 'verzonden'. Muteer tevens de urentegoeden conform de toelageresultaten. Van belang is dat elke periodeverantwoording in z'n geheel volledig wordt verwerkt. Het mag bijvoorbeeld niet voorkomen dat er toelageresultaten uit een periodeverantwoording naar P-Direkt gaan, terwijl de mutaties van urentegoeden vanuit diezelfde verantwoording niet verwerkt zijn.
+Verwijder aansluitend alle periodeverantwoordingen die NIET de status 'verzonden' hebben uit de overzichten in het startscherm, maar laat ze bestaan in de DTV-applicatie zodat SAS erbij kan. Ze worden pas verwijderd bij de volgende keer dat KNOP-1 wordt gebruikt.</t>
+  </si>
+  <si>
+    <t>Het consistent zijn van elke periodeverantwoording is van belang, zodat SAS altijd interpreteerbare gegevens ophaalt.</t>
+  </si>
+  <si>
+    <t>Het idee is dat dit signaal aan het datawarehouse er toe leidt, dat de medewerkers die te corrigeren periodeverantwoordingen hebben, daarvan in kennis worden gesteld. Vanuit de techniek is voorgesteld om de systeem-datum-en-tijd op te slaan in een record van de tabel applicatie-parameters.</t>
+  </si>
+  <si>
+    <t>Verwerk in kennismotor</t>
+  </si>
+  <si>
+    <t>Vrijgeven voor datawarehouse</t>
+  </si>
+  <si>
+    <t>KNOP-5</t>
+  </si>
+  <si>
+    <t>berekening</t>
+  </si>
+  <si>
+    <t>Achter de hyperlink bestaat er een Excel-bestand</t>
+  </si>
+  <si>
+    <t>Door het klikken op deze knop wordt Excel met daarin de onderbouwing van de periodeverantwoording aangeroepen. Editen van het bestand in Excel moet mogelijk zijn, maar opslaan van het gewijzigde resultaat in DTV niet.</t>
+  </si>
+  <si>
+    <t>De DTV-applicatie maakt de onderbouwing van berekeningen door de kennismotor beschikbaar voor de gebruiker. Voor elke opgeslagen periodeverantwoording die door KODE verwerkt is bestaat een XML-structuur, die door Excel direct leesbaar is. Omdat het opgeslagen Excel-bestand ook formules bevat, heeft de gebruiker de mogelijkheid om nog wat te "spelen" met deze verantwoording. Uiteraard mogen de resultaten daarvan niet terug naar de DTV-applicatie, want die slaat uitsluitend de verantwoording van de kennismotor zelf op.</t>
+  </si>
+  <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>DTV-107</t>
+  </si>
+  <si>
+    <t>DTV-104</t>
+  </si>
+  <si>
+    <t>DTV-109</t>
+  </si>
+  <si>
+    <t>voorverwerken</t>
+  </si>
+  <si>
+    <t>Verwijder alle periodeverantwoordingen die NIET de status 'verzonden' hebben, inclusief bijbehorende resultaten, uit DTV. Haal daarna de nieuwe batch op uit SPIN met daarin de geaccordeerde dagverantwoordingen, verdeel ze in periodeverantwoordingen en zet de status daarvan op 'te verwerken'.</t>
+  </si>
+  <si>
+    <t>KNOP-0</t>
+  </si>
+  <si>
+    <t>Verwijder alle periodeverantwoordingen die NIET de status 'verzonden' hebben, inclusief bijbehorende resultaten, uit DTV. Haal daarna de nieuwe batch op uit SPIN met daarin de definitieve dagverantwoordingen, verdeel ze in periodeverantwoordingen en zet de status daarvan op 'te verwerken'. De DTV-applicatie moet garanderen dat deze resultaten NIET naar P-Direkt worden verstuurd, noch enige mutatie van urentegoeden in de DTV-applicatie tot gevolg hebben.</t>
+  </si>
+  <si>
+    <t>Om teamleiders terugkoppeling te kunnen geven alvorens te accorderen, kunnen de tot dan toe definitief gemaakte dagverantwoordingen door de kennismotor worden verwerkt, zonder dat dit tot verwerking in DTV of P-Direkt leidt. De P&amp;O-medewerker kan zelf beslissen om deze mogelijkheid te gebruiken.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1003,7 +1066,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -1077,7 +1140,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1112,7 +1174,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -1288,24 +1349,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" customWidth="1"/>
-    <col min="4" max="4" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" customWidth="1"/>
+    <col min="4" max="4" width="64.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1328,7 +1389,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1348,7 +1409,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1368,7 +1429,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1388,7 +1449,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1405,7 +1466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1425,7 +1486,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1445,7 +1506,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1465,7 +1526,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1485,7 +1546,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -1502,7 +1563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -1519,7 +1580,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1534,7 +1595,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1551,7 +1612,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -1571,7 +1632,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1591,7 +1652,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1606,7 +1667,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1623,7 +1684,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>1</v>
       </c>
@@ -1643,7 +1704,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1660,7 +1721,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1680,7 +1741,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1697,7 +1758,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1705,7 +1766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -1722,7 +1783,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1742,7 +1803,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1756,7 +1817,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1773,7 +1834,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>62</v>
       </c>
@@ -1784,7 +1845,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>61</v>
       </c>
@@ -1805,23 +1866,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="6" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="48.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -1850,7 +1911,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -1876,7 +1937,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1902,7 +1963,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -1919,7 +1980,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>114</v>
       </c>
@@ -1942,7 +2003,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -1965,7 +2026,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -1985,7 +2046,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>90</v>
       </c>
@@ -1996,7 +2057,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>93</v>
       </c>
@@ -2019,7 +2080,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>94</v>
       </c>
@@ -2042,7 +2103,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>95</v>
       </c>
@@ -2065,7 +2126,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -2088,7 +2149,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>97</v>
       </c>
@@ -2111,7 +2172,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2134,7 +2195,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>100</v>
       </c>
@@ -2157,7 +2218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
         <v>101</v>
       </c>
@@ -2177,7 +2238,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>102</v>
       </c>
@@ -2197,7 +2258,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>103</v>
       </c>
@@ -2217,7 +2278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -2237,7 +2298,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -2257,7 +2318,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>104</v>
       </c>
@@ -2280,7 +2341,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -2300,7 +2361,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -2320,7 +2381,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -2340,7 +2401,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2357,7 +2418,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -2380,7 +2441,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>115</v>
       </c>
@@ -2403,7 +2464,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>117</v>
       </c>
@@ -2423,7 +2484,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -2443,7 +2504,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>119</v>
       </c>
@@ -2466,7 +2527,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>120</v>
       </c>
@@ -2486,7 +2547,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>121</v>
       </c>
@@ -2506,7 +2567,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>122</v>
       </c>
@@ -2526,7 +2587,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>123</v>
       </c>
@@ -2549,7 +2610,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>125</v>
       </c>
@@ -2572,7 +2633,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2595,7 +2656,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>129</v>
       </c>
@@ -2615,7 +2676,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>132</v>
       </c>
@@ -2635,7 +2696,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>133</v>
       </c>
@@ -2658,7 +2719,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
         <v>136</v>
       </c>
@@ -2681,7 +2742,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
         <v>138</v>
       </c>
@@ -2704,7 +2765,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="A42" t="s">
         <v>140</v>
       </c>
@@ -2727,7 +2788,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8">
       <c r="A43" t="s">
         <v>141</v>
       </c>
@@ -2750,7 +2811,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8">
       <c r="A44" t="s">
         <v>144</v>
       </c>
@@ -2773,7 +2834,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
         <v>146</v>
       </c>
@@ -2796,7 +2857,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8">
       <c r="A46" t="s">
         <v>148</v>
       </c>
@@ -2819,7 +2880,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8">
       <c r="A47" t="s">
         <v>151</v>
       </c>
@@ -2845,7 +2906,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8">
       <c r="A48" t="s">
         <v>93</v>
       </c>
@@ -2868,7 +2929,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" t="s">
         <v>154</v>
       </c>
@@ -2891,7 +2952,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -2920,7 +2981,7 @@
         <v>5010</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" t="s">
         <v>160</v>
       </c>
@@ -2946,7 +3007,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" t="s">
         <v>208</v>
       </c>
@@ -2969,7 +3030,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" t="s">
         <v>162</v>
       </c>
@@ -2992,7 +3053,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54" t="s">
         <v>163</v>
       </c>
@@ -3009,7 +3070,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55" t="s">
         <v>165</v>
       </c>
@@ -3032,7 +3093,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56" t="s">
         <v>167</v>
       </c>
@@ -3058,29 +3119,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="870" topLeftCell="A16" activePane="bottomLeft"/>
+      <pane ySplit="876" topLeftCell="A16" activePane="bottomLeft"/>
       <selection sqref="A1:XFD2"/>
       <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -3118,7 +3179,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -3150,7 +3211,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>216</v>
       </c>
@@ -3176,7 +3237,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>217</v>
       </c>
@@ -3202,7 +3263,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>221</v>
       </c>
@@ -3231,7 +3292,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>222</v>
       </c>
@@ -3260,7 +3321,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>209</v>
       </c>
@@ -3295,7 +3356,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>234</v>
       </c>
@@ -3327,7 +3388,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>234</v>
       </c>
@@ -3359,7 +3420,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>234</v>
       </c>
@@ -3391,7 +3452,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>234</v>
       </c>
@@ -3423,7 +3484,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>234</v>
       </c>
@@ -3455,7 +3516,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>226</v>
       </c>
@@ -3481,7 +3542,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>210</v>
       </c>
@@ -3513,7 +3574,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>213</v>
       </c>
@@ -3545,7 +3606,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -3580,7 +3641,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12">
       <c r="A19" t="s">
         <v>227</v>
       </c>
@@ -3609,7 +3670,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12">
       <c r="A20" t="s">
         <v>228</v>
       </c>
@@ -3638,7 +3699,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
       <c r="A21" t="s">
         <v>229</v>
       </c>
@@ -3667,7 +3728,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12">
       <c r="A23" t="s">
         <v>231</v>
       </c>
@@ -3702,7 +3763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12">
       <c r="A24" t="s">
         <v>231</v>
       </c>
@@ -3713,7 +3774,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12">
       <c r="A25" t="s">
         <v>158</v>
       </c>
@@ -3751,7 +3812,7 @@
         <v>5010</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12">
       <c r="A26" t="s">
         <v>160</v>
       </c>
@@ -3786,7 +3847,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12">
       <c r="A27" t="s">
         <v>208</v>
       </c>
@@ -3818,7 +3879,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12">
       <c r="A28" t="s">
         <v>233</v>
       </c>
@@ -3847,7 +3908,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12">
       <c r="A29" t="s">
         <v>165</v>
       </c>
@@ -3879,7 +3940,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12">
       <c r="A30" t="s">
         <v>167</v>
       </c>
@@ -3908,7 +3969,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12">
       <c r="A32" t="s">
         <v>240</v>
       </c>
@@ -3931,7 +3992,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="34" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11">
       <c r="B34" t="s">
         <v>185</v>
       </c>
@@ -3957,7 +4018,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11">
       <c r="B35" t="s">
         <v>185</v>
       </c>
@@ -3983,7 +4044,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11">
       <c r="B36" t="s">
         <v>185</v>
       </c>
@@ -4009,7 +4070,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11">
       <c r="B37" t="s">
         <v>185</v>
       </c>
@@ -4035,7 +4096,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11">
       <c r="B38" t="s">
         <v>185</v>
       </c>
@@ -4061,7 +4122,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="2:11" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11">
       <c r="B39" t="s">
         <v>185</v>
       </c>
@@ -4087,7 +4148,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:11">
       <c r="B40" t="s">
         <v>185</v>
       </c>
@@ -4113,7 +4174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:11">
       <c r="B42" t="s">
         <v>200</v>
       </c>
@@ -4139,7 +4200,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:11">
       <c r="B43" t="s">
         <v>200</v>
       </c>
@@ -4165,7 +4226,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11">
       <c r="B45" t="s">
         <v>201</v>
       </c>
@@ -4188,7 +4249,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11">
       <c r="B46" t="s">
         <v>201</v>
       </c>
@@ -4211,7 +4272,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11">
       <c r="B47" t="s">
         <v>202</v>
       </c>
@@ -4237,7 +4298,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:11">
       <c r="B48" t="s">
         <v>203</v>
       </c>
@@ -4260,7 +4321,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:11">
       <c r="B49" t="s">
         <v>203</v>
       </c>
@@ -4283,7 +4344,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:11">
       <c r="B50" t="s">
         <v>203</v>
       </c>
@@ -4306,7 +4367,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:11">
       <c r="B51" t="s">
         <v>203</v>
       </c>
@@ -4332,7 +4393,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:11">
       <c r="B52" t="s">
         <v>203</v>
       </c>
@@ -4358,7 +4419,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:11">
       <c r="B53" t="s">
         <v>203</v>
       </c>
@@ -4384,7 +4445,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:11">
       <c r="B55" t="s">
         <v>206</v>
       </c>
@@ -4410,7 +4471,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:11">
       <c r="B56" t="s">
         <v>206</v>
       </c>
@@ -4436,7 +4497,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:11">
       <c r="B57" t="s">
         <v>206</v>
       </c>
@@ -4462,7 +4523,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:11">
       <c r="B58" t="s">
         <v>206</v>
       </c>
@@ -4488,7 +4549,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:11">
       <c r="B59" t="s">
         <v>206</v>
       </c>
@@ -4514,7 +4575,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:11">
       <c r="B60" t="s">
         <v>206</v>
       </c>
@@ -4540,7 +4601,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:11">
       <c r="B61" t="s">
         <v>206</v>
       </c>
@@ -4574,24 +4635,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="32" style="4" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="4"/>
+    <col min="5" max="5" width="20.33203125" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>77</v>
       </c>
@@ -4605,10 +4666,10 @@
         <v>262</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="14.45" x14ac:dyDescent="0.3">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>77</v>
       </c>
@@ -4625,7 +4686,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="43.2">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -4642,7 +4703,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="43.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -4659,7 +4720,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="43.2">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -4676,7 +4737,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.2">
       <c r="A6" s="4" t="s">
         <v>244</v>
       </c>
@@ -4693,7 +4754,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="43.2">
       <c r="A7" s="4" t="s">
         <v>248</v>
       </c>
@@ -4717,129 +4778,223 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="40.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="40.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="37.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="58.5703125" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="40.5703125" style="4"/>
+    <col min="1" max="1" width="15.5546875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="37.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="39.88671875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="6.5546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="40.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="115.2">
+      <c r="A3" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="316.8">
+      <c r="A4" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="115.2">
+      <c r="A5" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="302.39999999999998">
+      <c r="A6" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="F3" s="5" t="s">
+      <c r="E6" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="H6" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="187.2">
+      <c r="A7" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="172.8">
+      <c r="A8" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>276</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>155</v>
+      <c r="H8" s="4" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tussentijdse commit voor Han
</commit_message>
<xml_diff>
--- a/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
+++ b/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="120" windowWidth="10500" windowHeight="9000"/>
+    <workbookView xWindow="288" yWindow="120" windowWidth="10500" windowHeight="9000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Schermen" sheetId="1" r:id="rId1"/>
     <sheet name="Interfaces 10 juni" sheetId="2" r:id="rId2"/>
     <sheet name="Gewenste Transacties" sheetId="3" r:id="rId3"/>
     <sheet name="Tabbladen" sheetId="4" r:id="rId4"/>
-    <sheet name="Knoppen" sheetId="5" r:id="rId5"/>
+    <sheet name="Functies" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_Toc411507377" localSheetId="0">Schermen!$F$25</definedName>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="377">
   <si>
     <t>Scherm</t>
   </si>
@@ -878,37 +878,10 @@
 Indien tijdens het verwerken op vernieuwen vanuit Spin wordt gedrukt, dan mag de kennismotor worden gestopt. Immers, zowel de nog niet verwerkte periodeverantwoordingen als ook de periodeverantwoordingen die door de kennismotor zijn verwerkt, zullen worden verwijderd.</t>
   </si>
   <si>
-    <t>activeringsEvent</t>
-  </si>
-  <si>
     <t>activeringsConditie</t>
   </si>
   <si>
-    <t>Event</t>
-  </si>
-  <si>
-    <t>Knop</t>
-  </si>
-  <si>
-    <t>[Knoppen]</t>
-  </si>
-  <si>
-    <t>KNOP-1</t>
-  </si>
-  <si>
-    <t>KNOP-2</t>
-  </si>
-  <si>
-    <t>KNOP-3</t>
-  </si>
-  <si>
     <t>Vernieuw alle periodeverantwoordingen</t>
-  </si>
-  <si>
-    <t>KNOP-4</t>
-  </si>
-  <si>
-    <t>Klik</t>
   </si>
   <si>
     <t>Het tijdstip van de klik wordt in een record opgeslagen, wat periodiek door SAS wordt uitgelezen. SAS stelt aan de hand van deze datum vast dat er nieuwe verantwoordingen klaarstaan. SAS zal de terugkoppelberichten voor medewerkers en teamleiders zelf uitlezen.</t>
@@ -930,9 +903,6 @@
     <t>Vrijgeven voor datawarehouse</t>
   </si>
   <si>
-    <t>KNOP-5</t>
-  </si>
-  <si>
     <t>berekening</t>
   </si>
   <si>
@@ -957,24 +927,15 @@
     <t>DTV-109</t>
   </si>
   <si>
-    <t>KNOP-6</t>
-  </si>
-  <si>
     <t>voorverwerken</t>
   </si>
   <si>
     <t>Verwijder alle periodeverantwoordingen die NIET de status 'verzonden' hebben, inclusief bijbehorende resultaten, uit DTV. Haal daarna de nieuwe batch op uit SPIN met daarin de geaccordeerde dagverantwoordingen, verdeel ze in periodeverantwoordingen en zet de status daarvan op 'te verwerken'.</t>
   </si>
   <si>
-    <t>KNOP-0</t>
-  </si>
-  <si>
     <t>Verwijder alle periodeverantwoordingen die NIET de status 'verzonden' hebben, inclusief bijbehorende resultaten, uit DTV. Haal daarna de nieuwe batch op uit SPIN met daarin de definitieve dagverantwoordingen, verdeel ze in periodeverantwoordingen en zet de status daarvan op 'te verwerken'. De DTV-applicatie moet garanderen dat deze resultaten NIET naar P-Direkt worden verstuurd, noch enige mutatie van urentegoeden in de DTV-applicatie tot gevolg hebben.</t>
   </si>
   <si>
-    <t>Om teamleiders terugkoppeling te kunnen geven alvorens te accorderen, kunnen de tot dan toe definitief gemaakte dagverantwoordingen door de kennismotor worden verwerkt, zonder dat dit tot verwerking in DTV of P-Direkt leidt. De P&amp;O-medewerker kan zelf beslissen om deze mogelijkheid te gebruiken.</t>
-  </si>
-  <si>
     <t>Er is tenminste één periodeverantwoording met de status 'te verwerken', en er is geen upload van P-Direktgegevens aan de gang.</t>
   </si>
   <si>
@@ -987,9 +948,6 @@
     <t xml:space="preserve">Lees van het aangeboden .xls-bestand de kolommen </t>
   </si>
   <si>
-    <t>KNOP-7</t>
-  </si>
-  <si>
     <t>DTV-86</t>
   </si>
   <si>
@@ -1015,6 +973,225 @@
   </si>
   <si>
     <t>lijst van perioderesultaten</t>
+  </si>
+  <si>
+    <t>Beheer &gt;  Arbeidsmodaliteiten Import</t>
+  </si>
+  <si>
+    <t>knop op Startpagina: Verwerk zonder opslaan</t>
+  </si>
+  <si>
+    <t>knop op Startpagina: Inladen geaccordeerde dagverantwoordingen</t>
+  </si>
+  <si>
+    <t>knop op Startpagina: Inladen definitieve dagverantwoordingen</t>
+  </si>
+  <si>
+    <t>knop op Startpagina: Vrijgeven van feedback</t>
+  </si>
+  <si>
+    <t>knop op Startpagina: Verstuur naar P-Direct</t>
+  </si>
+  <si>
+    <t>uiterlijk</t>
+  </si>
+  <si>
+    <t>actie</t>
+  </si>
+  <si>
+    <t>icoontje op of bij de combinatie van medewerker/verantwoordingsperiode</t>
+  </si>
+  <si>
+    <t>[Functies]</t>
+  </si>
+  <si>
+    <t>Fie-1</t>
+  </si>
+  <si>
+    <t>Fie-2</t>
+  </si>
+  <si>
+    <t>Fie-3</t>
+  </si>
+  <si>
+    <t>Fie-4</t>
+  </si>
+  <si>
+    <t>Fie-5</t>
+  </si>
+  <si>
+    <t>Fie-6</t>
+  </si>
+  <si>
+    <t>Fie-7</t>
+  </si>
+  <si>
+    <t>Fie-8</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t>obj</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Batchresultaat</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>CUD</t>
+  </si>
+  <si>
+    <t>proces</t>
+  </si>
+  <si>
+    <t>Proces</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>3e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wijzig urentegoed </t>
+  </si>
+  <si>
+    <t>het muteren van urentegoeden</t>
+  </si>
+  <si>
+    <t>het muteren van medewerkerrechten</t>
+  </si>
+  <si>
+    <t>het opvoeren van nieuwe medewerkers met hun categorie en salarisschaal</t>
+  </si>
+  <si>
+    <t>wijzig medewerkerrechten</t>
+  </si>
+  <si>
+    <t>DTV-113</t>
+  </si>
+  <si>
+    <t>DTV-102</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Stamgegeven</t>
+  </si>
+  <si>
+    <t>6b</t>
+  </si>
+  <si>
+    <t>6c</t>
+  </si>
+  <si>
+    <t>DTV-108</t>
+  </si>
+  <si>
+    <t>FO-DTV vs. 1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geïnformeerd accorderen door teamleiders </t>
+  </si>
+  <si>
+    <t xml:space="preserve">verantwoorden ten behoeve van Leidinggevenden en Control </t>
+  </si>
+  <si>
+    <t xml:space="preserve">het beheren van referentielijsten (stamtabellen) door een functioneel beheerder (FAB) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">het corrigeren met terugwerkende kracht van individuele registraties van urentegoeden en medewerkerrechten, wanneer administratieve fouten in het verleden dat noodzakelijk maken </t>
+  </si>
+  <si>
+    <t>FO-initiële gegevens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">corrigeer TWK urentegoed </t>
+  </si>
+  <si>
+    <t>upload urentegoeden</t>
+  </si>
+  <si>
+    <t>het corrigeren met terugwerkende kracht van alle registraties van medewerkerrechten vanaf een bepaalde datum door het inlezen van een Excel-bestand met de correcte gegevens.</t>
+  </si>
+  <si>
+    <t>het corrigeren met terugwerkende kracht van alle registraties van urentegoeden vanaf een bepaalde datum door het inlezen van een Excel-bestand met de correcte gegevens.</t>
+  </si>
+  <si>
+    <t>upload medewerkerrechten</t>
+  </si>
+  <si>
+    <t>via SAS</t>
+  </si>
+  <si>
+    <t>Beheer &gt; Referentielijsten</t>
+  </si>
+  <si>
+    <t>Fie-9</t>
+  </si>
+  <si>
+    <t>Fie-10</t>
+  </si>
+  <si>
+    <t>Fie-11</t>
+  </si>
+  <si>
+    <t>Fie-12</t>
+  </si>
+  <si>
+    <t>Fie-13</t>
+  </si>
+  <si>
+    <t>Fie-14</t>
+  </si>
+  <si>
+    <t>Fie-15</t>
+  </si>
+  <si>
+    <t>muteer stamgegevens</t>
+  </si>
+  <si>
+    <t>DTV1011</t>
+  </si>
+  <si>
+    <t>DTV9025</t>
+  </si>
+  <si>
+    <t>Beheer &gt; import arbeidsmodaliteiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Om teamleiders terugkoppeling te kunnen geven alvorens te accorderen, kunnen de tot dan toe definitief gemaakte dagverantwoordingen door de kennismotor worden verwerkt, zonder dat dit tot verwerking in DTV of P-Direkt leidt. De P&amp;O-medewerker kan zelf beslissen om deze mogelijkheid te gebruiken. Zolang er definitieve dagverantwoordingen in de periodebatch zitten,  is de knop "verstuur naar P-Direkt" niet aanwezig in de applicatie. </t>
   </si>
 </sst>
 </file>
@@ -1076,7 +1253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1089,6 +1266,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="10"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1389,10 +1575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1433,7 +1619,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>15</v>
@@ -1456,7 +1642,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>18</v>
@@ -1476,7 +1662,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>19</v>
@@ -1642,7 +1828,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1751,7 +1937,7 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>28</v>
@@ -1897,7 +2083,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="B29" t="s">
         <v>5</v>
@@ -1906,10 +2092,29 @@
         <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="E29" t="s">
-        <v>317</v>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>374</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>301</v>
+      </c>
+      <c r="D31" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -4835,40 +5040,44 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="37.44140625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="39.88671875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.88671875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.21875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="20.5546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="57.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="6.5546875" style="4" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="40.5546875" style="4"/>
+    <col min="9" max="9" width="42.21875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="8" customWidth="1"/>
+    <col min="12" max="16384" width="40.5546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
-        <v>276</v>
+        <v>313</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>263</v>
+        <v>310</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>264</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>265</v>
@@ -4877,18 +5086,21 @@
         <v>270</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B2" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="C2" s="4" t="s">
         <v>263</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>274</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>263</v>
@@ -4899,199 +5111,584 @@
       <c r="F2" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="115.2">
+      <c r="I2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="144">
       <c r="A3" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="100.8">
+      <c r="A4" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="216">
+      <c r="A5" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="86.4">
+      <c r="A6" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="244.8">
+      <c r="A7" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="129.6">
+      <c r="A8" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>300</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="E8" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H8" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="86.4">
+      <c r="A9" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="316.8">
-      <c r="A4" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="I9" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="100.8">
+      <c r="A10" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="G11" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28.8">
+      <c r="A12" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="43.2">
+      <c r="A13" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K13" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.8">
+      <c r="A15" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="43.2">
+      <c r="A16" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="28.8">
+      <c r="A17" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="C18" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="C19" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="115.2">
-      <c r="A5" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>288</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="302.39999999999998">
-      <c r="A6" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="187.2">
-      <c r="A7" s="4" t="s">
-        <v>289</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>290</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>292</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="172.8">
-      <c r="A8" s="4" t="s">
-        <v>301</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>303</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="57.6">
-      <c r="A9" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>307</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="115.2">
-      <c r="A10" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>311</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>282</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>313</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>310</v>
-      </c>
+      <c r="I19" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="K22" s="4"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="K23" s="4"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="K24" s="4"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="H25" s="6"/>
+      <c r="I25" s="9"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="K28" s="3"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="K30" s="4"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="L31" s="8"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="8"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="8"/>
+      <c r="Q31" s="8"/>
+      <c r="R31" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Stef, vind hier maar wat van!
</commit_message>
<xml_diff>
--- a/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
+++ b/NVWA DTV/werkdocumenten/Analyse Interfaces .xlsx
@@ -14,11 +14,11 @@
     <sheet name="Functies" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_Ref407429009" localSheetId="4">Functies!$L$13</definedName>
+    <definedName name="_Ref407429009" localSheetId="4">Functies!$L$14</definedName>
     <definedName name="_Toc411507377" localSheetId="0">Schermen!$F$25</definedName>
     <definedName name="_Toc411507378" localSheetId="0">Schermen!$F$26</definedName>
     <definedName name="_Toc411507379" localSheetId="0">Schermen!$F$6</definedName>
-    <definedName name="_Toc424111341" localSheetId="4">Functies!$L$13</definedName>
+    <definedName name="_Toc424111341" localSheetId="4">Functies!$L$14</definedName>
     <definedName name="_Toc424742519" localSheetId="4">Functies!$L$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1203" uniqueCount="390">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="392">
   <si>
     <t>Scherm</t>
   </si>
@@ -1267,6 +1267,12 @@
   </si>
   <si>
     <t xml:space="preserve">Indien er verantwoordingen worden geleverd met personeelsnummers die in de administratie van DTV nog niet voorkomen, dan dient er een nieuw personeelsnummer te worden aangemaakt. Indien bij deze aanlevering al een naam bekend is, dan wordt die hierin overgenomen. Hierdoor (en ook mogelijk andere manieren) kan het daardoor ontstaan, dat er medewerkers ontstaan, waarvoor geen salaris- en categorie is geregistreerd. </t>
+  </si>
+  <si>
+    <t>Beheren arbeidsmodaliteiten</t>
+  </si>
+  <si>
+    <t>het muteren van arbeidsmodaliteiten van een specifieke medewerker</t>
   </si>
 </sst>
 </file>
@@ -5123,11 +5129,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R32"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5395,7 +5401,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="91.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>312</v>
       </c>
@@ -5468,190 +5474,182 @@
         <v>379</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>357</v>
-      </c>
+    <row r="11" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>332</v>
+        <v>371</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>390</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="E11" s="11"/>
+        <v>391</v>
+      </c>
+      <c r="E11" s="6"/>
       <c r="G11" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H11" s="4" t="s">
-        <v>344</v>
-      </c>
       <c r="I11" s="4" t="s">
         <v>319</v>
       </c>
       <c r="J11" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="G12" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="J12" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="K11" s="7" t="s">
+      <c r="K12" s="7" t="s">
         <v>328</v>
       </c>
-      <c r="L11" s="8" t="s">
+      <c r="L12" s="8" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="E13" s="11"/>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>370</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>335</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="L13" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="102.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>336</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>334</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H14" s="8" t="s">
-        <v>337</v>
+      <c r="H14" s="4" t="s">
+        <v>344</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>319</v>
+        <v>154</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>229</v>
+        <v>40</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>330</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45.6" x14ac:dyDescent="0.3">
+        <v>329</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="102.6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>348</v>
+        <v>371</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>334</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>344</v>
+      <c r="H15" s="8" t="s">
+        <v>337</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>319</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>330</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="91.2" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="45.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>354</v>
+        <v>360</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>350</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>153</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>319</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>229</v>
+        <v>44</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="45.6" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="79.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>28</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>153</v>
@@ -5663,76 +5661,88 @@
         <v>319</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>331</v>
       </c>
       <c r="L17" s="8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="45.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="L18" s="8" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>347</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="8" t="s">
+      <c r="H19" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="L18" s="9" t="s">
+      <c r="L19" s="9" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="C19" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>346</v>
-      </c>
-      <c r="H19" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" ht="22.8" x14ac:dyDescent="0.3">
       <c r="C20" s="4" t="s">
         <v>355</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>284</v>
+        <v>343</v>
       </c>
       <c r="I20" s="4" t="s">
         <v>201</v>
@@ -5741,70 +5751,90 @@
         <v>209</v>
       </c>
       <c r="K20" s="7" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="C21" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>345</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="K21" s="7" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K24" s="4"/>
-      <c r="M24" s="6"/>
-      <c r="N24" s="6"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="H26" s="6"/>
-      <c r="I26" s="11"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K26" s="4"/>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="L26" s="8"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="H27" s="6"/>
+      <c r="I27" s="11"/>
       <c r="K27" s="4"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K28" s="4"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="K29" s="8"/>
-      <c r="O29" s="8"/>
-      <c r="P29" s="8"/>
-      <c r="Q29" s="8"/>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="K30" s="4"/>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K30" s="8"/>
+      <c r="O30" s="8"/>
+      <c r="P30" s="8"/>
+      <c r="Q30" s="8"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="K31" s="4"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="7"/>
-      <c r="N32" s="7"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="K32" s="4"/>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>